<commit_message>
added apache poi instruments to iport/export items for all language classes
</commit_message>
<xml_diff>
--- a/src/main/resources/users.xlsx
+++ b/src/main/resources/users.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
-    <sheet name="Items" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -46,9 +45,6 @@
     <t>Sukiasyan</t>
   </si>
   <si>
-    <t>AS077778752</t>
-  </si>
-  <si>
     <t>aram1995</t>
   </si>
   <si>
@@ -58,13 +54,16 @@
     <t>Surenyan</t>
   </si>
   <si>
-    <t>SS077885566</t>
-  </si>
-  <si>
     <t>suren1990</t>
   </si>
   <si>
     <t>male</t>
+  </si>
+  <si>
+    <t>077778752</t>
+  </si>
+  <si>
+    <t>077778899</t>
   </si>
 </sst>
 </file>
@@ -109,9 +108,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -394,92 +397,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="15.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="22" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified import/export methods items for all language classes
</commit_message>
<xml_diff>
--- a/src/main/resources/users.xlsx
+++ b/src/main/resources/users.xlsx
@@ -7,7 +7,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="English" sheetId="1" r:id="rId1"/>
+    <sheet name="Հայերեն" sheetId="2" r:id="rId2"/>
+    <sheet name="Русский" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,25 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>surname</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Aram</t>
   </si>
@@ -64,6 +48,90 @@
   </si>
   <si>
     <t>077778899</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Անուն</t>
+  </si>
+  <si>
+    <t>Ազգանուն</t>
+  </si>
+  <si>
+    <t>Սեռ</t>
+  </si>
+  <si>
+    <t>Տարիք</t>
+  </si>
+  <si>
+    <t>Հեռ. Համար</t>
+  </si>
+  <si>
+    <t>Գաղտնաբառ</t>
+  </si>
+  <si>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>Фамилия</t>
+  </si>
+  <si>
+    <t>Пол</t>
+  </si>
+  <si>
+    <t>Возраст</t>
+  </si>
+  <si>
+    <t>Тел. Номер</t>
+  </si>
+  <si>
+    <t>Пароль</t>
+  </si>
+  <si>
+    <t>Արամ</t>
+  </si>
+  <si>
+    <t>Սուքիասյան</t>
+  </si>
+  <si>
+    <t>Արական</t>
+  </si>
+  <si>
+    <t>Սուրեն</t>
+  </si>
+  <si>
+    <t>Սուրենյան</t>
+  </si>
+  <si>
+    <t>Арам</t>
+  </si>
+  <si>
+    <t>Сукиасян</t>
+  </si>
+  <si>
+    <t>Мужской</t>
+  </si>
+  <si>
+    <t>Сурен</t>
+  </si>
+  <si>
+    <t>Суренян</t>
   </si>
 </sst>
 </file>
@@ -412,62 +480,62 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="3">
         <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3">
         <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -477,4 +545,177 @@
     <ignoredError sqref="E2:E3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="15.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="22" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="3">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E3" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="15.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="22" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="3">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>